<commit_message>
0.0.1: Now blancoPinia is released.
</commit_message>
<xml_diff>
--- a/meta/stores/SampleNoGettersStore.xlsx
+++ b/meta/stores/SampleNoGettersStore.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoPinia/meta/stores/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{862FF410-5FD3-D246-9E1C-6D51AE5A70C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3341B4D7-026C-7240-A7A0-D7C59328F2D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="72">
   <si>
     <t>パッケージ</t>
   </si>
@@ -505,38 +505,7 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>updateState01</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>void</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>state01 の値を更新します。</t>
-    <rPh sb="9" eb="10">
-      <t xml:space="preserve">アタイヲ </t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t xml:space="preserve">コウシｎ </t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>value</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>state01 の新しい値です。</t>
-    <rPh sb="8" eb="9">
-      <t>ノ</t>
-    </rPh>
-    <rPh sb="9" eb="10">
-      <t xml:space="preserve">アタラシイ </t>
-    </rPh>
-    <rPh sb="12" eb="13">
-      <t xml:space="preserve">アタイデス。 </t>
-    </rPh>
     <phoneticPr fontId="3"/>
   </si>
   <si>
@@ -1883,8 +1852,8 @@
   </sheetPr>
   <dimension ref="A1:K98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1933,7 +1902,7 @@
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="8"/>
@@ -1948,7 +1917,7 @@
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="10" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D7" s="33"/>
       <c r="E7" s="11"/>
@@ -1993,7 +1962,7 @@
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="109" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D10" s="110"/>
       <c r="E10" s="111"/>
@@ -2058,7 +2027,7 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="30" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B15" s="31"/>
       <c r="C15" s="31"/>
@@ -2278,7 +2247,7 @@
         <v>34</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F28" s="20"/>
       <c r="G28" s="20" t="s">
@@ -2360,7 +2329,7 @@
     </row>
     <row r="35" spans="1:11">
       <c r="A35" s="30" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B35" s="31"/>
       <c r="C35" s="31"/>
@@ -2795,7 +2764,7 @@
     </row>
     <row r="68" spans="1:11">
       <c r="A68" s="30" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B68" s="31"/>
       <c r="C68" s="31"/>
@@ -2928,7 +2897,7 @@
         <v>6</v>
       </c>
       <c r="F77" s="100" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G77" s="92" t="s">
         <v>1</v>
@@ -2955,18 +2924,12 @@
       <c r="A79" s="19">
         <v>1</v>
       </c>
-      <c r="B79" s="70" t="s">
-        <v>60</v>
-      </c>
-      <c r="C79" s="86" t="s">
-        <v>61</v>
-      </c>
+      <c r="B79" s="70"/>
+      <c r="C79" s="86"/>
       <c r="D79" s="89"/>
       <c r="E79" s="83"/>
       <c r="F79" s="68"/>
-      <c r="G79" s="20" t="s">
-        <v>62</v>
-      </c>
+      <c r="G79" s="20"/>
       <c r="H79" s="21"/>
       <c r="I79" s="21"/>
       <c r="J79" s="28"/>
@@ -2977,18 +2940,12 @@
         <f>A79+1</f>
         <v>2</v>
       </c>
-      <c r="B80" s="70" t="s">
-        <v>63</v>
-      </c>
-      <c r="C80" s="86" t="s">
-        <v>29</v>
-      </c>
+      <c r="B80" s="70"/>
+      <c r="C80" s="86"/>
       <c r="D80" s="89"/>
       <c r="E80" s="83"/>
       <c r="F80" s="68"/>
-      <c r="G80" s="20" t="s">
-        <v>64</v>
-      </c>
+      <c r="G80" s="20"/>
       <c r="H80" s="21"/>
       <c r="I80" s="21"/>
       <c r="J80" s="28"/>
@@ -3113,7 +3070,7 @@
         <v>6</v>
       </c>
       <c r="F90" s="100" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G90" s="102" t="s">
         <v>1</v>
@@ -3141,7 +3098,7 @@
         <v>1</v>
       </c>
       <c r="B92" s="70" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C92" s="86" t="s">
         <v>34</v>
@@ -3152,7 +3109,7 @@
         <v>14</v>
       </c>
       <c r="G92" s="20" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="H92" s="21"/>
       <c r="I92" s="21"/>
@@ -3165,7 +3122,7 @@
         <v>2</v>
       </c>
       <c r="B93" s="70" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C93" s="86" t="s">
         <v>34</v>
@@ -3174,7 +3131,7 @@
       <c r="E93" s="83"/>
       <c r="F93" s="68"/>
       <c r="G93" s="20" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H93" s="21"/>
       <c r="I93" s="21"/>

</xml_diff>